<commit_message>
Update Db and evaluation results
</commit_message>
<xml_diff>
--- a/new_classification_db/N10 - REQUIREMENTS.xlsx
+++ b/new_classification_db/N10 - REQUIREMENTS.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="171">
   <si>
     <t xml:space="preserve">NOTIFICATION TYPE</t>
   </si>
@@ -389,6 +389,12 @@
   </si>
   <si>
     <t xml:space="preserve">MANIFIESTE LO QUE A SU DERECHO CONVENGA RESPECTO A LA APLICACIÓN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARA QUE CONFIRME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LAS CANTIDADES</t>
   </si>
   <si>
     <t xml:space="preserve">N10 - FULL REQUIREMENT SPECIFICATION</t>
@@ -672,10 +678,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z65536"/>
+  <dimension ref="A1:Z157"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A116" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B136" activeCellId="0" sqref="B136"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A111" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D119" activeCellId="0" sqref="D119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -683,8 +689,9 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.668016194332"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="71.7692307692308"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="1.39271255060729"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="26" min="5" style="0" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.6923076923077"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.4493927125506"/>
+    <col collapsed="false" hidden="false" max="26" min="6" style="0" width="10.6032388663968"/>
     <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="14.6761133603239"/>
   </cols>
   <sheetData>
@@ -1922,66 +1929,86 @@
       <c r="Z118" s="3"/>
     </row>
     <row r="119" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A119" s="3" t="s">
+      <c r="A119" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B119" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="B119" s="3" t="s">
+      <c r="C119" s="3"/>
+      <c r="D119" s="3" t="s">
         <v>124</v>
       </c>
+      <c r="E119" s="3"/>
+      <c r="F119" s="3"/>
+      <c r="G119" s="3"/>
+      <c r="H119" s="3"/>
+      <c r="I119" s="3"/>
+      <c r="J119" s="3"/>
+      <c r="K119" s="3"/>
+      <c r="L119" s="3"/>
+      <c r="M119" s="3"/>
+      <c r="N119" s="3"/>
+      <c r="O119" s="3"/>
+      <c r="P119" s="3"/>
+      <c r="Q119" s="3"/>
+      <c r="R119" s="3"/>
+      <c r="S119" s="3"/>
+      <c r="T119" s="3"/>
+      <c r="U119" s="3"/>
+      <c r="V119" s="3"/>
+      <c r="W119" s="3"/>
+      <c r="X119" s="3"/>
+      <c r="Y119" s="3"/>
+      <c r="Z119" s="3"/>
     </row>
     <row r="120" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B120" s="0" t="s">
         <v>125</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="D121" s="0" t="s">
         <v>127</v>
-      </c>
-      <c r="F121" s="0" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B122" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="D122" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="C122" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D122" s="0" t="s">
-        <v>73</v>
+      <c r="F122" s="0" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B123" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="C123" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D123" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B123" s="0" t="s">
         <v>131</v>
+      </c>
+      <c r="C123" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D123" s="0" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B124" s="6" t="s">
         <v>132</v>
@@ -1995,7 +2022,7 @@
     </row>
     <row r="125" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B125" s="6" t="s">
         <v>134</v>
@@ -2006,70 +2033,73 @@
       <c r="D125" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="E125" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="F125" s="0" t="s">
-        <v>136</v>
-      </c>
     </row>
     <row r="126" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B126" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C126" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D126" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="C126" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D126" s="6" t="s">
+      <c r="E126" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F126" s="0" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A127" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B127" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B127" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="C127" s="4"/>
-      <c r="D127" s="4"/>
-      <c r="E127" s="4"/>
+      <c r="C127" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D127" s="6" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="128" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="C128" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D128" s="4" t="s">
         <v>141</v>
       </c>
+      <c r="C128" s="4"/>
+      <c r="D128" s="4"/>
       <c r="E128" s="4"/>
     </row>
     <row r="129" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A129" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B129" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C129" s="4"/>
-      <c r="D129" s="4"/>
+      <c r="C129" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D129" s="4" t="s">
+        <v>143</v>
+      </c>
       <c r="E129" s="4"/>
     </row>
     <row r="130" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C130" s="4"/>
       <c r="D130" s="4"/>
@@ -2077,10 +2107,10 @@
     </row>
     <row r="131" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C131" s="4"/>
       <c r="D131" s="4"/>
@@ -2088,36 +2118,36 @@
     </row>
     <row r="132" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C132" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D132" s="4" t="s">
         <v>146</v>
       </c>
+      <c r="C132" s="4"/>
+      <c r="D132" s="4"/>
       <c r="E132" s="4"/>
     </row>
     <row r="133" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B133" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="C133" s="4"/>
-      <c r="D133" s="4"/>
+      <c r="C133" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D133" s="4" t="s">
+        <v>148</v>
+      </c>
       <c r="E133" s="4"/>
     </row>
     <row r="134" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C134" s="4"/>
       <c r="D134" s="4"/>
@@ -2125,10 +2155,10 @@
     </row>
     <row r="135" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C135" s="4"/>
       <c r="D135" s="4"/>
@@ -2136,74 +2166,49 @@
     </row>
     <row r="136" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C136" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D136" s="4" t="s">
-        <v>149</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="C136" s="4"/>
+      <c r="D136" s="4"/>
       <c r="E136" s="4"/>
     </row>
     <row r="137" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A137" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B137" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C137" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D137" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="E137" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F137" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="G137" s="3"/>
-      <c r="H137" s="3"/>
-      <c r="I137" s="3"/>
-      <c r="J137" s="3"/>
-      <c r="K137" s="3"/>
-      <c r="L137" s="3"/>
-      <c r="M137" s="3"/>
-      <c r="N137" s="3"/>
-      <c r="O137" s="3"/>
-      <c r="P137" s="3"/>
-      <c r="Q137" s="3"/>
-      <c r="R137" s="3"/>
-      <c r="S137" s="3"/>
-      <c r="T137" s="3"/>
-      <c r="U137" s="3"/>
-      <c r="V137" s="3"/>
-      <c r="W137" s="3"/>
-      <c r="X137" s="3"/>
-      <c r="Y137" s="3"/>
-      <c r="Z137" s="3"/>
+      <c r="A137" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C137" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D137" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="E137" s="4"/>
     </row>
     <row r="138" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="5" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="C138" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D138" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="E138" s="3"/>
-      <c r="F138" s="3"/>
+        <v>129</v>
+      </c>
+      <c r="E138" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F138" s="5" t="s">
+        <v>152</v>
+      </c>
       <c r="G138" s="3"/>
       <c r="H138" s="3"/>
       <c r="I138" s="3"/>
@@ -2227,13 +2232,17 @@
     </row>
     <row r="139" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A139" s="5" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B139" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="C139" s="3"/>
-      <c r="D139" s="3"/>
+        <v>139</v>
+      </c>
+      <c r="C139" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D139" s="5" t="s">
+        <v>153</v>
+      </c>
       <c r="E139" s="3"/>
       <c r="F139" s="3"/>
       <c r="G139" s="3"/>
@@ -2259,15 +2268,13 @@
     </row>
     <row r="140" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="5" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B140" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C140" s="3"/>
-      <c r="D140" s="3" t="s">
-        <v>47</v>
-      </c>
+      <c r="D140" s="3"/>
       <c r="E140" s="3"/>
       <c r="F140" s="3"/>
       <c r="G140" s="3"/>
@@ -2292,10 +2299,16 @@
       <c r="Z140" s="3"/>
     </row>
     <row r="141" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A141" s="5"/>
-      <c r="B141" s="5"/>
+      <c r="A141" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B141" s="5" t="s">
+        <v>155</v>
+      </c>
       <c r="C141" s="3"/>
-      <c r="D141" s="3"/>
+      <c r="D141" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="E141" s="3"/>
       <c r="F141" s="3"/>
       <c r="G141" s="3"/>
@@ -2320,16 +2333,36 @@
       <c r="Z141" s="3"/>
     </row>
     <row r="142" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A142" s="7" t="s">
-        <v>154</v>
-      </c>
+      <c r="A142" s="5"/>
+      <c r="B142" s="5"/>
+      <c r="C142" s="3"/>
+      <c r="D142" s="3"/>
+      <c r="E142" s="3"/>
+      <c r="F142" s="3"/>
+      <c r="G142" s="3"/>
+      <c r="H142" s="3"/>
+      <c r="I142" s="3"/>
+      <c r="J142" s="3"/>
+      <c r="K142" s="3"/>
+      <c r="L142" s="3"/>
+      <c r="M142" s="3"/>
+      <c r="N142" s="3"/>
+      <c r="O142" s="3"/>
+      <c r="P142" s="3"/>
+      <c r="Q142" s="3"/>
+      <c r="R142" s="3"/>
+      <c r="S142" s="3"/>
+      <c r="T142" s="3"/>
+      <c r="U142" s="3"/>
+      <c r="V142" s="3"/>
+      <c r="W142" s="3"/>
+      <c r="X142" s="3"/>
+      <c r="Y142" s="3"/>
+      <c r="Z142" s="3"/>
     </row>
     <row r="143" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A143" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B143" s="0" t="s">
-        <v>155</v>
+      <c r="A143" s="7" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2337,7 +2370,7 @@
         <v>2</v>
       </c>
       <c r="B144" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2345,7 +2378,7 @@
         <v>2</v>
       </c>
       <c r="B145" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2353,7 +2386,7 @@
         <v>2</v>
       </c>
       <c r="B146" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2361,7 +2394,7 @@
         <v>2</v>
       </c>
       <c r="B147" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2369,7 +2402,7 @@
         <v>2</v>
       </c>
       <c r="B148" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2377,7 +2410,7 @@
         <v>2</v>
       </c>
       <c r="B149" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2385,7 +2418,7 @@
         <v>2</v>
       </c>
       <c r="B150" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2393,7 +2426,7 @@
         <v>2</v>
       </c>
       <c r="B151" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2401,7 +2434,7 @@
         <v>2</v>
       </c>
       <c r="B152" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2409,7 +2442,7 @@
         <v>2</v>
       </c>
       <c r="B153" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2417,7 +2450,7 @@
         <v>2</v>
       </c>
       <c r="B154" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2425,7 +2458,7 @@
         <v>2</v>
       </c>
       <c r="B155" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2433,10 +2466,17 @@
         <v>2</v>
       </c>
       <c r="B156" s="0" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>169</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A157" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B157" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>